<commit_message>
pre and post graphs
</commit_message>
<xml_diff>
--- a/Data/Pre and Post/Pre_Post_Stacked.xlsx
+++ b/Data/Pre and Post/Pre_Post_Stacked.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/oliviarandell/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/oliviarandell/Documents/GitHub/GGEESummer23/Data/Pre and Post/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92432A88-764A-9446-B7B8-2AB261874788}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F8AC346-4A2A-3749-BCD1-E7FE05FA1F97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14460" yWindow="500" windowWidth="12660" windowHeight="15940" firstSheet="1" activeTab="2" xr2:uid="{DE2E1B36-43E4-254A-A049-873EBAF2C466}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="618" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="618" uniqueCount="44">
   <si>
     <t>Experience</t>
   </si>
@@ -146,10 +146,34 @@
     <t>How would you rate your coding skills?</t>
   </si>
   <si>
-    <t>Prior to the summer camp</t>
-  </si>
-  <si>
-    <t>After the Summer Camp</t>
+    <t>0-None</t>
+  </si>
+  <si>
+    <t>1-Basic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2-Medium </t>
+  </si>
+  <si>
+    <t>3-High</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pre- Summer Program </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Post- Summer Program </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1-No experience </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2-A little experience </t>
+  </si>
+  <si>
+    <t xml:space="preserve">3-Some experience </t>
+  </si>
+  <si>
+    <t>4-A lot of experience</t>
   </si>
 </sst>
 </file>
@@ -3913,7 +3937,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3937,7 +3961,7 @@
         <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>15</v>
+        <v>40</v>
       </c>
       <c r="C2">
         <v>18</v>
@@ -3951,7 +3975,7 @@
         <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>41</v>
       </c>
       <c r="C3">
         <v>48</v>
@@ -3965,7 +3989,7 @@
         <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>42</v>
       </c>
       <c r="C4">
         <v>48</v>
@@ -3979,7 +4003,7 @@
         <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>2</v>
+        <v>43</v>
       </c>
       <c r="C5">
         <v>23</v>
@@ -3998,7 +4022,7 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4029,10 +4053,10 @@
         <v>33</v>
       </c>
       <c r="B2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" t="s">
         <v>34</v>
-      </c>
-      <c r="C2" t="s">
-        <v>19</v>
       </c>
       <c r="D2">
         <v>28</v>
@@ -4046,10 +4070,10 @@
         <v>33</v>
       </c>
       <c r="B3" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="C3" t="s">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="D3">
         <v>67</v>
@@ -4063,10 +4087,10 @@
         <v>33</v>
       </c>
       <c r="B4" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="C4" t="s">
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="D4">
         <v>33</v>
@@ -4080,10 +4104,10 @@
         <v>33</v>
       </c>
       <c r="B5" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="C5" t="s">
-        <v>22</v>
+        <v>37</v>
       </c>
       <c r="D5">
         <v>9</v>
@@ -4097,10 +4121,10 @@
         <v>33</v>
       </c>
       <c r="B6" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="C6" t="s">
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="D6">
         <v>4</v>
@@ -4114,10 +4138,10 @@
         <v>33</v>
       </c>
       <c r="B7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7" t="s">
         <v>35</v>
-      </c>
-      <c r="C7" t="s">
-        <v>20</v>
       </c>
       <c r="D7">
         <v>18</v>
@@ -4131,10 +4155,10 @@
         <v>33</v>
       </c>
       <c r="B8" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="C8" t="s">
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="D8">
         <v>75</v>
@@ -4148,10 +4172,10 @@
         <v>33</v>
       </c>
       <c r="B9" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="C9" t="s">
-        <v>22</v>
+        <v>37</v>
       </c>
       <c r="D9">
         <v>40</v>

</xml_diff>